<commit_message>
push selenium with pom
</commit_message>
<xml_diff>
--- a/src/test/resources/data/Adactin.xlsx
+++ b/src/test/resources/data/Adactin.xlsx
@@ -4,13 +4,16 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="16095" windowHeight="7365" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="16095" windowHeight="7365"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
-    <sheet name="Login" sheetId="1" r:id="rId2"/>
-    <sheet name="HotelBookingData" sheetId="2" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="8" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="6" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
+    <sheet name="Login" sheetId="1" r:id="rId4"/>
+    <sheet name="HotelBookingData" sheetId="2" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="5" r:id="rId6"/>
+    <sheet name="Sheet4" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="125725"/>
   <extLst>
@@ -30,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="21">
   <si>
     <t>username</t>
   </si>
@@ -75,6 +78,24 @@
   </si>
   <si>
     <t>2 - Two</t>
+  </si>
+  <si>
+    <t>adultsPerRoom</t>
+  </si>
+  <si>
+    <t>childrenPerRoom</t>
+  </si>
+  <si>
+    <t>expectedFinalPrice</t>
+  </si>
+  <si>
+    <t>1 - One</t>
+  </si>
+  <si>
+    <t>0 - None</t>
+  </si>
+  <si>
+    <t>expectedTotalPrice</t>
   </si>
 </sst>
 </file>
@@ -647,6 +668,187 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:L1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="7">
+        <v>45874</v>
+      </c>
+      <c r="H2" s="4">
+        <v>45905</v>
+      </c>
+      <c r="I2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="7">
+        <v>45874</v>
+      </c>
+      <c r="H2" s="4">
+        <v>45905</v>
+      </c>
+      <c r="I2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -723,7 +925,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -762,7 +964,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H2"/>
   <sheetViews>
@@ -837,11 +1039,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
@@ -913,4 +1115,107 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="7">
+        <v>45874</v>
+      </c>
+      <c r="H2" s="4">
+        <v>45905</v>
+      </c>
+      <c r="I2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2">
+        <v>125</v>
+      </c>
+      <c r="L2">
+        <v>135</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>